<commit_message>
ok hasta tabla segun concejo comunitario
</commit_message>
<xml_diff>
--- a/public/reportes/reporte_caracterizacion.xlsx
+++ b/public/reportes/reporte_caracterizacion.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="89">
   <si>
     <t>MACROPROCESO: AGENCIA NACIONAL DE TIERRAS 
 PROCESO: DIRECCIÓN DE ASUNTOS ÉTNICOS</t>
@@ -40,7 +40,7 @@
     <t>2. Municipio: EL PASO</t>
   </si>
   <si>
-    <t>3. Corregimiento o vereda:   La Loma de Calenturas</t>
+    <t>3. Corregimiento o vereda:   Consolidado General</t>
   </si>
   <si>
     <t>4. Fecha: 14 de Noviembre del 2023</t>
@@ -119,69 +119,123 @@
     <t>Area Utilizada</t>
   </si>
   <si>
+    <t>Fabian Andres Quintero Mendez</t>
+  </si>
+  <si>
+    <t>CC</t>
+  </si>
+  <si>
+    <t>Masculino</t>
+  </si>
+  <si>
+    <t>22 Años</t>
+  </si>
+  <si>
+    <t>Unión Libre</t>
+  </si>
+  <si>
+    <t>Jefe de hogar</t>
+  </si>
+  <si>
+    <t>Desempleado Buscando empleo</t>
+  </si>
+  <si>
+    <t>analfabeta</t>
+  </si>
+  <si>
+    <t>Parcela</t>
+  </si>
+  <si>
+    <t>Propia</t>
+  </si>
+  <si>
+    <t>Si</t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t>Juan Camilo Quiñones</t>
+  </si>
+  <si>
+    <t>TI</t>
+  </si>
+  <si>
+    <t>17 Años</t>
+  </si>
+  <si>
+    <t>Soltero</t>
+  </si>
+  <si>
+    <t>Hijastro(a)</t>
+  </si>
+  <si>
+    <t>Estudiante</t>
+  </si>
+  <si>
+    <t>cursando primaria</t>
+  </si>
+  <si>
+    <t>Juana de arcos</t>
+  </si>
+  <si>
+    <t>Femenino</t>
+  </si>
+  <si>
+    <t>20 Años</t>
+  </si>
+  <si>
+    <t>Yerno(a)</t>
+  </si>
+  <si>
+    <t>Modisto</t>
+  </si>
+  <si>
+    <t>Daniela Quintero</t>
+  </si>
+  <si>
+    <t>18 Años</t>
+  </si>
+  <si>
+    <t>Desempleado Sin Busqueda de Empleo</t>
+  </si>
+  <si>
+    <t>Universitario incompleto</t>
+  </si>
+  <si>
+    <t>Finca</t>
+  </si>
+  <si>
     <t>Obdulio Josefino Gaviria</t>
   </si>
   <si>
-    <t>CC</t>
-  </si>
-  <si>
-    <t>Masculino</t>
-  </si>
-  <si>
     <t>58 Años</t>
   </si>
   <si>
     <t>Viudo(a)</t>
   </si>
   <si>
-    <t>Jefe de hogar</t>
-  </si>
-  <si>
     <t>Agricultor cultivador</t>
   </si>
   <si>
     <t>sin estudios</t>
   </si>
   <si>
-    <t>Finca</t>
-  </si>
-  <si>
-    <t>Propia</t>
-  </si>
-  <si>
-    <t>No</t>
-  </si>
-  <si>
-    <t>Si</t>
-  </si>
-  <si>
     <t>Andres gaviria</t>
   </si>
   <si>
-    <t>TI</t>
-  </si>
-  <si>
     <t>3 Años</t>
   </si>
   <si>
-    <t>Soltero</t>
-  </si>
-  <si>
     <t>Hijo(a)</t>
   </si>
   <si>
-    <t>Desempleado Sin Busqueda de Empleo</t>
-  </si>
-  <si>
     <t>cursando Bachillerato</t>
   </si>
   <si>
     <t>Juana Gaviria</t>
   </si>
   <si>
-    <t>Femenino</t>
-  </si>
-  <si>
     <t>38 Años</t>
   </si>
   <si>
@@ -194,15 +248,6 @@
     <t>Cocinero de restaurante</t>
   </si>
   <si>
-    <t>Daniela Quintero</t>
-  </si>
-  <si>
-    <t>18 Años</t>
-  </si>
-  <si>
-    <t>Universitario incompleto</t>
-  </si>
-  <si>
     <t>Miguel Ángel López</t>
   </si>
   <si>
@@ -230,7 +275,19 @@
     <t>NO APLICA</t>
   </si>
   <si>
-    <t>analfabeta</t>
+    <t>Andrea Madrid</t>
+  </si>
+  <si>
+    <t>36 Años</t>
+  </si>
+  <si>
+    <t>Ayudante de cocina no domestica</t>
+  </si>
+  <si>
+    <t>bachillerato completo</t>
+  </si>
+  <si>
+    <t>Alquilada</t>
   </si>
 </sst>
 </file>
@@ -674,10 +731,10 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:Z13"/>
+  <dimension ref="A1:Z17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
-      <selection activeCell="S12" sqref="S12:S13"/>
+      <selection activeCell="S17" sqref="S17:S17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -695,7 +752,7 @@
     <col min="11" max="11" width="20" customWidth="true" style="0"/>
     <col min="12" max="12" width="25" customWidth="true" style="0"/>
     <col min="13" max="13" width="10.569" bestFit="true" customWidth="true" style="0"/>
-    <col min="14" max="14" width="10.569" bestFit="true" customWidth="true" style="0"/>
+    <col min="14" max="14" width="12.568" bestFit="true" customWidth="true" style="0"/>
     <col min="15" max="15" width="10.569" bestFit="true" customWidth="true" style="0"/>
     <col min="16" max="16" width="12.568" bestFit="true" customWidth="true" style="0"/>
     <col min="17" max="17" width="10.283" bestFit="true" customWidth="true" style="0"/>
@@ -936,7 +993,7 @@
         <v>33</v>
       </c>
       <c r="F8" s="1">
-        <v>10090908978.0</v>
+        <v>134543433.0</v>
       </c>
       <c r="G8" s="1" t="s">
         <v>34</v>
@@ -969,13 +1026,13 @@
         <v>43</v>
       </c>
       <c r="Q8" s="1">
-        <v>200000</v>
+        <v>15000</v>
       </c>
       <c r="R8" s="1">
-        <v>20.0</v>
+        <v>1.5</v>
       </c>
       <c r="S8" s="1">
-        <v>70000.0</v>
+        <v>11000.0</v>
       </c>
     </row>
     <row r="9" spans="1:26" customHeight="1" ht="30">
@@ -991,7 +1048,7 @@
         <v>45</v>
       </c>
       <c r="F9" s="1">
-        <v>100212124.0</v>
+        <v>23123123123.0</v>
       </c>
       <c r="G9" s="1" t="s">
         <v>34</v>
@@ -1032,7 +1089,7 @@
         <v>33</v>
       </c>
       <c r="F10" s="1">
-        <v>4234234234.0</v>
+        <v>7547546546.0</v>
       </c>
       <c r="G10" s="1" t="s">
         <v>52</v>
@@ -1041,13 +1098,13 @@
         <v>53</v>
       </c>
       <c r="I10" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="J10" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="J10" s="1" t="s">
+      <c r="K10" s="2" t="s">
         <v>55</v>
-      </c>
-      <c r="K10" s="2" t="s">
-        <v>56</v>
       </c>
       <c r="L10" s="2" t="s">
         <v>39</v>
@@ -1068,7 +1125,7 @@
         <v>1</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D11" s="1"/>
       <c r="E11" s="1" t="s">
@@ -1081,7 +1138,7 @@
         <v>52</v>
       </c>
       <c r="H11" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="I11" s="1" t="s">
         <v>47</v>
@@ -1090,22 +1147,22 @@
         <v>37</v>
       </c>
       <c r="K11" s="2" t="s">
-        <v>49</v>
+        <v>58</v>
       </c>
       <c r="L11" s="2" t="s">
         <v>59</v>
       </c>
       <c r="M11" s="1" t="s">
-        <v>40</v>
+        <v>60</v>
       </c>
       <c r="N11" s="1" t="s">
         <v>41</v>
       </c>
       <c r="O11" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="P11" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="Q11" s="1">
         <v>50000</v>
@@ -1125,53 +1182,53 @@
         <v>1</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="D12" s="1"/>
       <c r="E12" s="1" t="s">
         <v>33</v>
       </c>
       <c r="F12" s="1">
-        <v>213412321321.0</v>
+        <v>10090908978.0</v>
       </c>
       <c r="G12" s="1" t="s">
         <v>34</v>
       </c>
       <c r="H12" s="1" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="I12" s="1" t="s">
-        <v>47</v>
+        <v>63</v>
       </c>
       <c r="J12" s="1" t="s">
         <v>37</v>
       </c>
       <c r="K12" s="2" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="L12" s="2" t="s">
-        <v>59</v>
+        <v>65</v>
       </c>
       <c r="M12" s="1" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="N12" s="1" t="s">
         <v>41</v>
       </c>
       <c r="O12" s="1" t="s">
-        <v>64</v>
+        <v>43</v>
       </c>
       <c r="P12" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="Q12" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="R12" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="S12" s="1" t="s">
-        <v>64</v>
+        <v>42</v>
+      </c>
+      <c r="Q12" s="1">
+        <v>200000</v>
+      </c>
+      <c r="R12" s="1">
+        <v>20.0</v>
+      </c>
+      <c r="S12" s="1">
+        <v>70000.0</v>
       </c>
     </row>
     <row r="13" spans="1:26" customHeight="1" ht="30">
@@ -1180,29 +1237,29 @@
         <v>2</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="D13" s="1"/>
       <c r="E13" s="1" t="s">
-        <v>33</v>
+        <v>45</v>
       </c>
       <c r="F13" s="1">
-        <v>42324234234.0</v>
+        <v>100212124.0</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>52</v>
+        <v>34</v>
       </c>
       <c r="H13" s="1" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="I13" s="1" t="s">
-        <v>36</v>
+        <v>47</v>
       </c>
       <c r="J13" s="1" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="K13" s="2" t="s">
-        <v>68</v>
+        <v>58</v>
       </c>
       <c r="L13" s="2" t="s">
         <v>69</v>
@@ -1214,6 +1271,202 @@
       <c r="Q13" s="1"/>
       <c r="R13" s="1"/>
       <c r="S13" s="1"/>
+    </row>
+    <row r="14" spans="1:26" customHeight="1" ht="30">
+      <c r="A14" s="1"/>
+      <c r="B14" s="1">
+        <v>3</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="D14" s="1"/>
+      <c r="E14" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="F14" s="1">
+        <v>4234234234.0</v>
+      </c>
+      <c r="G14" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="H14" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="I14" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="J14" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="K14" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="L14" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="M14" s="1"/>
+      <c r="N14" s="1"/>
+      <c r="O14" s="1"/>
+      <c r="P14" s="1"/>
+      <c r="Q14" s="1"/>
+      <c r="R14" s="1"/>
+      <c r="S14" s="1"/>
+    </row>
+    <row r="15" spans="1:26" customHeight="1" ht="30">
+      <c r="A15" s="1">
+        <v>4</v>
+      </c>
+      <c r="B15" s="1">
+        <v>1</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="D15" s="1"/>
+      <c r="E15" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="F15" s="1">
+        <v>213412321321.0</v>
+      </c>
+      <c r="G15" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="H15" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="I15" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="J15" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="K15" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="L15" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="M15" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="N15" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="O15" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="P15" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="Q15" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="R15" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="S15" s="1" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="16" spans="1:26" customHeight="1" ht="30">
+      <c r="A16" s="1"/>
+      <c r="B16" s="1">
+        <v>2</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="D16" s="1"/>
+      <c r="E16" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="F16" s="1">
+        <v>42324234234.0</v>
+      </c>
+      <c r="G16" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="H16" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="I16" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="J16" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="K16" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="L16" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="M16" s="1"/>
+      <c r="N16" s="1"/>
+      <c r="O16" s="1"/>
+      <c r="P16" s="1"/>
+      <c r="Q16" s="1"/>
+      <c r="R16" s="1"/>
+      <c r="S16" s="1"/>
+    </row>
+    <row r="17" spans="1:26" customHeight="1" ht="30">
+      <c r="A17" s="1">
+        <v>5</v>
+      </c>
+      <c r="B17" s="1">
+        <v>1</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="D17" s="1"/>
+      <c r="E17" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="F17" s="1">
+        <v>967897897.0</v>
+      </c>
+      <c r="G17" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="H17" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="I17" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="J17" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="K17" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="L17" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="M17" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="N17" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="O17" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="P17" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="Q17" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="R17" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="S17" s="1" t="s">
+        <v>79</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells>
@@ -1241,6 +1494,10 @@
     <mergeCell ref="C11:D11"/>
     <mergeCell ref="C12:D12"/>
     <mergeCell ref="C13:D13"/>
+    <mergeCell ref="C14:D14"/>
+    <mergeCell ref="C15:D15"/>
+    <mergeCell ref="C16:D16"/>
+    <mergeCell ref="C17:D17"/>
     <mergeCell ref="A8:A10"/>
     <mergeCell ref="M8:M10"/>
     <mergeCell ref="N8:N10"/>
@@ -1257,14 +1514,30 @@
     <mergeCell ref="Q11:Q11"/>
     <mergeCell ref="R11:R11"/>
     <mergeCell ref="S11:S11"/>
-    <mergeCell ref="A12:A13"/>
-    <mergeCell ref="M12:M13"/>
-    <mergeCell ref="N12:N13"/>
-    <mergeCell ref="O12:O13"/>
-    <mergeCell ref="P12:P13"/>
-    <mergeCell ref="Q12:Q13"/>
-    <mergeCell ref="R12:R13"/>
-    <mergeCell ref="S12:S13"/>
+    <mergeCell ref="A12:A14"/>
+    <mergeCell ref="M12:M14"/>
+    <mergeCell ref="N12:N14"/>
+    <mergeCell ref="O12:O14"/>
+    <mergeCell ref="P12:P14"/>
+    <mergeCell ref="Q12:Q14"/>
+    <mergeCell ref="R12:R14"/>
+    <mergeCell ref="S12:S14"/>
+    <mergeCell ref="A15:A16"/>
+    <mergeCell ref="M15:M16"/>
+    <mergeCell ref="N15:N16"/>
+    <mergeCell ref="O15:O16"/>
+    <mergeCell ref="P15:P16"/>
+    <mergeCell ref="Q15:Q16"/>
+    <mergeCell ref="R15:R16"/>
+    <mergeCell ref="S15:S16"/>
+    <mergeCell ref="A17:A17"/>
+    <mergeCell ref="M17:M17"/>
+    <mergeCell ref="N17:N17"/>
+    <mergeCell ref="O17:O17"/>
+    <mergeCell ref="P17:P17"/>
+    <mergeCell ref="Q17:Q17"/>
+    <mergeCell ref="R17:R17"/>
+    <mergeCell ref="S17:S17"/>
   </mergeCells>
   <printOptions gridLines="false" gridLinesSet="true"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
ok poblacion activa e inactiva
</commit_message>
<xml_diff>
--- a/public/reportes/reporte_caracterizacion.xlsx
+++ b/public/reportes/reporte_caracterizacion.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="102">
   <si>
     <t>MACROPROCESO: AGENCIA NACIONAL DE TIERRAS 
 PROCESO: DIRECCIÓN DE ASUNTOS ÉTNICOS</t>
@@ -46,10 +46,10 @@
     <t>4. Fecha: 14 de Noviembre del 2023</t>
   </si>
   <si>
-    <t>5. Representante Legal: EUFROSINA VEGA MIELES</t>
-  </si>
-  <si>
-    <t>6. Consejo Comunitario: Consejo Comunitario  Julio Cesar Altamar Muñoz</t>
+    <t xml:space="preserve">5. Representante Legal: </t>
+  </si>
+  <si>
+    <t>6. Consejo Comunitario: Todos</t>
   </si>
   <si>
     <t>Listado de Personas</t>
@@ -315,6 +315,18 @@
   </si>
   <si>
     <t>Alquilada</t>
+  </si>
+  <si>
+    <t>Andres Jose Madrid Madrid</t>
+  </si>
+  <si>
+    <t>Registro Civil</t>
+  </si>
+  <si>
+    <t>5 Años</t>
+  </si>
+  <si>
+    <t>No Aplica</t>
   </si>
 </sst>
 </file>
@@ -761,10 +773,10 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:Z18"/>
+  <dimension ref="A1:Z19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
-      <selection activeCell="S18" sqref="S18:S18"/>
+      <selection activeCell="S18" sqref="S18:S19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -772,7 +784,7 @@
     <col min="1" max="1" width="13.568" bestFit="true" customWidth="true" style="0"/>
     <col min="2" max="2" width="11.569" bestFit="true" customWidth="true" style="0"/>
     <col min="3" max="3" width="33.992" bestFit="true" customWidth="true" style="0"/>
-    <col min="4" max="4" width="7.284" bestFit="true" customWidth="true" style="0"/>
+    <col min="4" max="4" width="17.853" bestFit="true" customWidth="true" style="0"/>
     <col min="5" max="5" width="15.853" bestFit="true" customWidth="true" style="0"/>
     <col min="6" max="6" width="41.561" bestFit="true" customWidth="true" style="0"/>
     <col min="7" max="7" width="12.568" bestFit="true" customWidth="true" style="0"/>
@@ -1562,6 +1574,49 @@
       <c r="S18" s="1" t="s">
         <v>89</v>
       </c>
+    </row>
+    <row r="19" spans="1:26" customHeight="1" ht="30">
+      <c r="A19" s="1"/>
+      <c r="B19" s="1">
+        <v>2</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="E19" s="10">
+        <v>523423454.0</v>
+      </c>
+      <c r="F19" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="G19" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="H19" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="I19" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="J19" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="K19" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="L19" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="M19" s="1"/>
+      <c r="N19" s="1"/>
+      <c r="O19" s="1"/>
+      <c r="P19" s="1"/>
+      <c r="Q19" s="1"/>
+      <c r="R19" s="1"/>
+      <c r="S19" s="1"/>
     </row>
   </sheetData>
   <mergeCells>
@@ -1614,14 +1669,14 @@
     <mergeCell ref="Q16:Q17"/>
     <mergeCell ref="R16:R17"/>
     <mergeCell ref="S16:S17"/>
-    <mergeCell ref="A18:A18"/>
-    <mergeCell ref="M18:M18"/>
-    <mergeCell ref="N18:N18"/>
-    <mergeCell ref="O18:O18"/>
-    <mergeCell ref="P18:P18"/>
-    <mergeCell ref="Q18:Q18"/>
-    <mergeCell ref="R18:R18"/>
-    <mergeCell ref="S18:S18"/>
+    <mergeCell ref="A18:A19"/>
+    <mergeCell ref="M18:M19"/>
+    <mergeCell ref="N18:N19"/>
+    <mergeCell ref="O18:O19"/>
+    <mergeCell ref="P18:P19"/>
+    <mergeCell ref="Q18:Q19"/>
+    <mergeCell ref="R18:R19"/>
+    <mergeCell ref="S18:S19"/>
   </mergeCells>
   <printOptions gridLines="false" gridLinesSet="true"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
ok segunda pantalla de informes
</commit_message>
<xml_diff>
--- a/public/reportes/reporte_caracterizacion.xlsx
+++ b/public/reportes/reporte_caracterizacion.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="102">
   <si>
     <t>MACROPROCESO: AGENCIA NACIONAL DE TIERRAS 
 PROCESO: DIRECCIÓN DE ASUNTOS ÉTNICOS</t>
@@ -161,24 +161,69 @@
     <t>No</t>
   </si>
   <si>
+    <t>Juan Camilo Quiñones</t>
+  </si>
+  <si>
+    <t>TI</t>
+  </si>
+  <si>
+    <t>17 Años</t>
+  </si>
+  <si>
+    <t>Soltero</t>
+  </si>
+  <si>
+    <t>Hijastro(a)</t>
+  </si>
+  <si>
+    <t>Estudiante</t>
+  </si>
+  <si>
+    <t>Cursando primaria</t>
+  </si>
+  <si>
+    <t>Juana de arcos</t>
+  </si>
+  <si>
+    <t>Femenino</t>
+  </si>
+  <si>
+    <t>20 Años</t>
+  </si>
+  <si>
+    <t>Yerno(a)</t>
+  </si>
+  <si>
+    <t>Modisto</t>
+  </si>
+  <si>
+    <t>Bachillerato completo</t>
+  </si>
+  <si>
+    <t>Juan Jole Lopez</t>
+  </si>
+  <si>
+    <t>2 Años</t>
+  </si>
+  <si>
+    <t>Nieto(a)</t>
+  </si>
+  <si>
+    <t>NO APLICA</t>
+  </si>
+  <si>
+    <t>Sin estudios</t>
+  </si>
+  <si>
     <t>Daniela Quintero</t>
   </si>
   <si>
-    <t>TI</t>
-  </si>
-  <si>
     <t>manzana 12 casa 18 - Primero de mayo</t>
   </si>
   <si>
-    <t>Femenino</t>
-  </si>
-  <si>
     <t>18 Años</t>
   </si>
   <si>
-    <t>Soltero</t>
-  </si>
-  <si>
     <t>Desempleado Sin Busqueda de Empleo</t>
   </si>
   <si>
@@ -203,7 +248,31 @@
     <t>Agricultor cultivador</t>
   </si>
   <si>
-    <t>Sin estudios</t>
+    <t>Andres gaviria</t>
+  </si>
+  <si>
+    <t>3 Años</t>
+  </si>
+  <si>
+    <t>Hijo(a)</t>
+  </si>
+  <si>
+    <t>Cursando Bachillerato</t>
+  </si>
+  <si>
+    <t>Juana Gaviria</t>
+  </si>
+  <si>
+    <t>38 Años</t>
+  </si>
+  <si>
+    <t>Divorciado</t>
+  </si>
+  <si>
+    <t>Hermano(a)</t>
+  </si>
+  <si>
+    <t>Cocinero de restaurante</t>
   </si>
   <si>
     <t>Miguel Ángel López</t>
@@ -224,6 +293,15 @@
     <t>N.A</t>
   </si>
   <si>
+    <t>Abuela Miguel Angel</t>
+  </si>
+  <si>
+    <t>83 Años</t>
+  </si>
+  <si>
+    <t>Abuelo(a)</t>
+  </si>
+  <si>
     <t>Andrea Madrid</t>
   </si>
   <si>
@@ -236,10 +314,19 @@
     <t>Ayudante de cocina no domestica</t>
   </si>
   <si>
-    <t>Bachillerato completo</t>
-  </si>
-  <si>
     <t>Alquilada</t>
+  </si>
+  <si>
+    <t>Andres Jose Madrid Madrid</t>
+  </si>
+  <si>
+    <t>Registro Civil</t>
+  </si>
+  <si>
+    <t>5 Años</t>
+  </si>
+  <si>
+    <t>No Aplica</t>
   </si>
 </sst>
 </file>
@@ -686,10 +773,10 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:Z12"/>
+  <dimension ref="A1:Z19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
-      <selection activeCell="S12" sqref="S12"/>
+      <selection activeCell="S18" sqref="S18:S19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -697,7 +784,7 @@
     <col min="1" max="1" width="13.568" bestFit="true" customWidth="true" style="0"/>
     <col min="2" max="2" width="11.569" bestFit="true" customWidth="true" style="0"/>
     <col min="3" max="3" width="33.992" bestFit="true" customWidth="true" style="0"/>
-    <col min="4" max="4" width="7.284" bestFit="true" customWidth="true" style="0"/>
+    <col min="4" max="4" width="17.853" bestFit="true" customWidth="true" style="0"/>
     <col min="5" max="5" width="15.853" bestFit="true" customWidth="true" style="0"/>
     <col min="6" max="6" width="41.561" bestFit="true" customWidth="true" style="0"/>
     <col min="7" max="7" width="12.568" bestFit="true" customWidth="true" style="0"/>
@@ -995,11 +1082,9 @@
       </c>
     </row>
     <row r="9" spans="1:26" customHeight="1" ht="30">
-      <c r="A9" s="1">
+      <c r="A9" s="1"/>
+      <c r="B9" s="1">
         <v>2</v>
-      </c>
-      <c r="B9" s="1">
-        <v>1</v>
       </c>
       <c r="C9" s="2" t="s">
         <v>46</v>
@@ -1008,227 +1093,530 @@
         <v>47</v>
       </c>
       <c r="E9" s="10">
-        <v>43423423423.0</v>
+        <v>23123123123.0</v>
       </c>
       <c r="F9" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="G9" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="H9" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="G9" s="1" t="s">
+      <c r="I9" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="H9" s="1" t="s">
+      <c r="J9" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="I9" s="1" t="s">
+      <c r="K9" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="J9" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="K9" s="2" t="s">
+      <c r="L9" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="L9" s="2" t="s">
+      <c r="M9" s="1"/>
+      <c r="N9" s="1"/>
+      <c r="O9" s="1"/>
+      <c r="P9" s="1"/>
+      <c r="Q9" s="1"/>
+      <c r="R9" s="1"/>
+      <c r="S9" s="1"/>
+    </row>
+    <row r="10" spans="1:26" customHeight="1" ht="30">
+      <c r="A10" s="1"/>
+      <c r="B10" s="1">
+        <v>3</v>
+      </c>
+      <c r="C10" s="2" t="s">
         <v>53</v>
-      </c>
-      <c r="M9" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="N9" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="O9" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="P9" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="Q9" s="1">
-        <v>50000</v>
-      </c>
-      <c r="R9" s="1">
-        <v>5.0</v>
-      </c>
-      <c r="S9" s="1">
-        <v>47000.0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:26" customHeight="1" ht="30">
-      <c r="A10" s="1">
-        <v>3</v>
-      </c>
-      <c r="B10" s="1">
-        <v>1</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>55</v>
       </c>
       <c r="D10" s="1" t="s">
         <v>34</v>
       </c>
       <c r="E10" s="10">
-        <v>10090908978.0</v>
+        <v>7547546546.0</v>
       </c>
       <c r="F10" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="G10" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="H10" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="I10" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="J10" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="G10" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="H10" s="1" t="s">
+      <c r="K10" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="I10" s="1" t="s">
+      <c r="L10" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="J10" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="K10" s="2" t="s">
+      <c r="M10" s="1"/>
+      <c r="N10" s="1"/>
+      <c r="O10" s="1"/>
+      <c r="P10" s="1"/>
+      <c r="Q10" s="1"/>
+      <c r="R10" s="1"/>
+      <c r="S10" s="1"/>
+    </row>
+    <row r="11" spans="1:26" customHeight="1" ht="30">
+      <c r="A11" s="1"/>
+      <c r="B11" s="1">
+        <v>4</v>
+      </c>
+      <c r="C11" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="L10" s="2" t="s">
+      <c r="D11" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="E11" s="10">
+        <v>432423423.0</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="G11" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="H11" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="M10" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="N10" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="O10" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="P10" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="Q10" s="1">
-        <v>200000</v>
-      </c>
-      <c r="R10" s="1">
-        <v>20.0</v>
-      </c>
-      <c r="S10" s="1">
-        <v>70000.0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:26" customHeight="1" ht="30">
-      <c r="A11" s="1">
-        <v>4</v>
-      </c>
-      <c r="B11" s="1">
-        <v>1</v>
-      </c>
-      <c r="C11" s="2" t="s">
+      <c r="I11" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="J11" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="D11" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="E11" s="10">
-        <v>213412321321.0</v>
-      </c>
-      <c r="F11" s="1" t="s">
+      <c r="K11" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="G11" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="H11" s="1" t="s">
+      <c r="L11" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="I11" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="J11" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="K11" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="L11" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="M11" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="N11" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="O11" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="P11" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="Q11" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="R11" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="S11" s="1" t="s">
-        <v>66</v>
-      </c>
+      <c r="M11" s="1"/>
+      <c r="N11" s="1"/>
+      <c r="O11" s="1"/>
+      <c r="P11" s="1"/>
+      <c r="Q11" s="1"/>
+      <c r="R11" s="1"/>
+      <c r="S11" s="1"/>
     </row>
     <row r="12" spans="1:26" customHeight="1" ht="30">
       <c r="A12" s="1">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="B12" s="1">
         <v>1</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>34</v>
+        <v>47</v>
       </c>
       <c r="E12" s="10">
-        <v>967897897.0</v>
+        <v>43423423423.0</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="G12" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="H12" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="I12" s="1" t="s">
         <v>49</v>
-      </c>
-      <c r="H12" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="I12" s="1" t="s">
-        <v>51</v>
       </c>
       <c r="J12" s="1" t="s">
         <v>39</v>
       </c>
       <c r="K12" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="L12" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="M12" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="N12" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="O12" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="P12" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="Q12" s="1">
+        <v>50000</v>
+      </c>
+      <c r="R12" s="1">
+        <v>5.0</v>
+      </c>
+      <c r="S12" s="1">
+        <v>47000.0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:26" customHeight="1" ht="30">
+      <c r="A13" s="1">
+        <v>3</v>
+      </c>
+      <c r="B13" s="1">
+        <v>1</v>
+      </c>
+      <c r="C13" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="L12" s="2" t="s">
+      <c r="D13" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="E13" s="10">
+        <v>10090908978.0</v>
+      </c>
+      <c r="F13" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="M12" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="N12" s="1" t="s">
+      <c r="G13" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="H13" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="O12" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="P12" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="Q12" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="R12" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="S12" s="1" t="s">
-        <v>66</v>
-      </c>
+      <c r="I13" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="J13" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="K13" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="L13" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="M13" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="N13" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="O13" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="P13" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="Q13" s="1">
+        <v>200000</v>
+      </c>
+      <c r="R13" s="1">
+        <v>20.0</v>
+      </c>
+      <c r="S13" s="1">
+        <v>70000.0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:26" customHeight="1" ht="30">
+      <c r="A14" s="1"/>
+      <c r="B14" s="1">
+        <v>2</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="E14" s="10">
+        <v>100212124.0</v>
+      </c>
+      <c r="F14" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="G14" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="H14" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="I14" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="J14" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="K14" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="L14" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="M14" s="1"/>
+      <c r="N14" s="1"/>
+      <c r="O14" s="1"/>
+      <c r="P14" s="1"/>
+      <c r="Q14" s="1"/>
+      <c r="R14" s="1"/>
+      <c r="S14" s="1"/>
+    </row>
+    <row r="15" spans="1:26" customHeight="1" ht="30">
+      <c r="A15" s="1"/>
+      <c r="B15" s="1">
+        <v>3</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="E15" s="10">
+        <v>4234234234.0</v>
+      </c>
+      <c r="F15" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="G15" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="H15" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="I15" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="J15" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="K15" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="L15" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="M15" s="1"/>
+      <c r="N15" s="1"/>
+      <c r="O15" s="1"/>
+      <c r="P15" s="1"/>
+      <c r="Q15" s="1"/>
+      <c r="R15" s="1"/>
+      <c r="S15" s="1"/>
+    </row>
+    <row r="16" spans="1:26" customHeight="1" ht="30">
+      <c r="A16" s="1">
+        <v>4</v>
+      </c>
+      <c r="B16" s="1">
+        <v>1</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="E16" s="10">
+        <v>213412321321.0</v>
+      </c>
+      <c r="F16" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="G16" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="H16" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="I16" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="J16" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="K16" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="L16" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="M16" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="N16" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="O16" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="P16" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="Q16" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="R16" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="S16" s="1" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="17" spans="1:26" customHeight="1" ht="30">
+      <c r="A17" s="1"/>
+      <c r="B17" s="1">
+        <v>2</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="E17" s="10">
+        <v>42324234234.0</v>
+      </c>
+      <c r="F17" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="G17" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="H17" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="I17" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="J17" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="K17" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="L17" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="M17" s="1"/>
+      <c r="N17" s="1"/>
+      <c r="O17" s="1"/>
+      <c r="P17" s="1"/>
+      <c r="Q17" s="1"/>
+      <c r="R17" s="1"/>
+      <c r="S17" s="1"/>
+    </row>
+    <row r="18" spans="1:26" customHeight="1" ht="30">
+      <c r="A18" s="1">
+        <v>5</v>
+      </c>
+      <c r="B18" s="1">
+        <v>1</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="E18" s="10">
+        <v>967897897.0</v>
+      </c>
+      <c r="F18" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="G18" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="H18" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="I18" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="J18" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="K18" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="L18" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="M18" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="N18" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="O18" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="P18" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="Q18" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="R18" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="S18" s="1" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="19" spans="1:26" customHeight="1" ht="30">
+      <c r="A19" s="1"/>
+      <c r="B19" s="1">
+        <v>2</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="E19" s="10">
+        <v>523423454.0</v>
+      </c>
+      <c r="F19" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="G19" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="H19" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="I19" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="J19" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="K19" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="L19" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="M19" s="1"/>
+      <c r="N19" s="1"/>
+      <c r="O19" s="1"/>
+      <c r="P19" s="1"/>
+      <c r="Q19" s="1"/>
+      <c r="R19" s="1"/>
+      <c r="S19" s="1"/>
     </row>
   </sheetData>
   <mergeCells>
@@ -1249,6 +1637,46 @@
     <mergeCell ref="G6:L6"/>
     <mergeCell ref="M6:N6"/>
     <mergeCell ref="O6:S6"/>
+    <mergeCell ref="A8:A11"/>
+    <mergeCell ref="M8:M11"/>
+    <mergeCell ref="N8:N11"/>
+    <mergeCell ref="O8:O11"/>
+    <mergeCell ref="P8:P11"/>
+    <mergeCell ref="Q8:Q11"/>
+    <mergeCell ref="R8:R11"/>
+    <mergeCell ref="S8:S11"/>
+    <mergeCell ref="A12:A12"/>
+    <mergeCell ref="M12:M12"/>
+    <mergeCell ref="N12:N12"/>
+    <mergeCell ref="O12:O12"/>
+    <mergeCell ref="P12:P12"/>
+    <mergeCell ref="Q12:Q12"/>
+    <mergeCell ref="R12:R12"/>
+    <mergeCell ref="S12:S12"/>
+    <mergeCell ref="A13:A15"/>
+    <mergeCell ref="M13:M15"/>
+    <mergeCell ref="N13:N15"/>
+    <mergeCell ref="O13:O15"/>
+    <mergeCell ref="P13:P15"/>
+    <mergeCell ref="Q13:Q15"/>
+    <mergeCell ref="R13:R15"/>
+    <mergeCell ref="S13:S15"/>
+    <mergeCell ref="A16:A17"/>
+    <mergeCell ref="M16:M17"/>
+    <mergeCell ref="N16:N17"/>
+    <mergeCell ref="O16:O17"/>
+    <mergeCell ref="P16:P17"/>
+    <mergeCell ref="Q16:Q17"/>
+    <mergeCell ref="R16:R17"/>
+    <mergeCell ref="S16:S17"/>
+    <mergeCell ref="A18:A19"/>
+    <mergeCell ref="M18:M19"/>
+    <mergeCell ref="N18:N19"/>
+    <mergeCell ref="O18:O19"/>
+    <mergeCell ref="P18:P19"/>
+    <mergeCell ref="Q18:Q19"/>
+    <mergeCell ref="R18:R19"/>
+    <mergeCell ref="S18:S19"/>
   </mergeCells>
   <printOptions gridLines="false" gridLinesSet="true"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>